<commit_message>
updated fem% master spreadsheet
</commit_message>
<xml_diff>
--- a/src/results/Faulkner-Fem-Percent-Spreadsheet.xlsx
+++ b/src/results/Faulkner-Fem-Percent-Spreadsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="faulkner-fem-percent-no-names" sheetId="1" r:id="rId1"/>
@@ -1060,11 +1060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="492947248"/>
-        <c:axId val="492943328"/>
+        <c:axId val="363146416"/>
+        <c:axId val="363144064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="492947248"/>
+        <c:axId val="363146416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492943328"/>
+        <c:crossAx val="363144064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1115,7 +1115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492943328"/>
+        <c:axId val="363144064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,7 +1166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492947248"/>
+        <c:crossAx val="363146416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1486,11 +1486,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="497836560"/>
-        <c:axId val="497838128"/>
+        <c:axId val="363147984"/>
+        <c:axId val="335333064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497836560"/>
+        <c:axId val="363147984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497838128"/>
+        <c:crossAx val="335333064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1541,7 +1541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497838128"/>
+        <c:axId val="335333064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497836560"/>
+        <c:crossAx val="363147984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1656,6 +1656,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fem% (strict)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1887,11 +1912,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="554680680"/>
-        <c:axId val="554682248"/>
+        <c:axId val="335336592"/>
+        <c:axId val="335333848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="554680680"/>
+        <c:axId val="335336592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="554682248"/>
+        <c:crossAx val="335333848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1942,7 +1967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="554682248"/>
+        <c:axId val="335333848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -1994,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="554680680"/>
+        <c:crossAx val="335336592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4032,9 +4057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>